<commit_message>
Rewrite the RScripts/Venue_Analytics.R with bug fix; Speed improvement to parser Now the analytics computes D1 trade flows
</commit_message>
<xml_diff>
--- a/RScripts/Trade_Flow_Summary.xlsx
+++ b/RScripts/Trade_Flow_Summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="35">
   <si>
     <t>A Listed</t>
   </si>
@@ -104,6 +104,24 @@
   <si>
     <t>%</t>
   </si>
+  <si>
+    <t>CSCO</t>
+  </si>
+  <si>
+    <t>imegrp</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>YHOO</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -229,11 +247,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -258,6 +356,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3647,12 +3759,1613 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="16">
+        <v>12750</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>2300</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="18">
+        <v>15318</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>28403</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="18">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>300</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="18">
+        <v>190961</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>646238</v>
+      </c>
+      <c r="K6" s="1">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>95193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="18">
+        <v>67085</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>132546</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>24102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="18">
+        <v>47522</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>31702</v>
+      </c>
+      <c r="K8" s="1">
+        <v>6</v>
+      </c>
+      <c r="L8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="18">
+        <v>47406</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>124770</v>
+      </c>
+      <c r="K9" s="1">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>62901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="18">
+        <v>500</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>218015</v>
+      </c>
+      <c r="K10" s="1">
+        <v>8</v>
+      </c>
+      <c r="L10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>69672</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="18">
+        <v>52858</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>468288</v>
+      </c>
+      <c r="K11" s="1">
+        <v>9</v>
+      </c>
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <v>94273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="18">
+        <v>148400</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>1500</v>
+      </c>
+      <c r="K12" s="1">
+        <v>10</v>
+      </c>
+      <c r="L12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="18">
+        <v>800</v>
+      </c>
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>22205</v>
+      </c>
+      <c r="K13" s="1">
+        <v>11</v>
+      </c>
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="18">
+        <v>300</v>
+      </c>
+      <c r="F14" s="1">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>7640</v>
+      </c>
+      <c r="K14" s="1">
+        <v>12</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>6866</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="18">
+        <v>11339</v>
+      </c>
+      <c r="F15" s="1">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>257788</v>
+      </c>
+      <c r="K15" s="1">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>13901</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
+        <v>14</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="21">
+        <v>123951</v>
+      </c>
+      <c r="F16" s="1">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <v>3400</v>
+      </c>
+      <c r="K16" s="1">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>15</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="16">
+        <v>14740</v>
+      </c>
+      <c r="F17" s="1">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17">
+        <v>148421</v>
+      </c>
+      <c r="K17" s="1">
+        <v>15</v>
+      </c>
+      <c r="L17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N17">
+        <v>23166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18">
+        <v>58397</v>
+      </c>
+      <c r="F18" s="1">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <v>200</v>
+      </c>
+      <c r="K18" s="1">
+        <v>16</v>
+      </c>
+      <c r="L18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M18" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="18">
+        <v>400</v>
+      </c>
+      <c r="F19" s="1">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <v>653192</v>
+      </c>
+      <c r="K19" s="1">
+        <v>17</v>
+      </c>
+      <c r="L19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" t="s">
+        <v>15</v>
+      </c>
+      <c r="N19">
+        <v>150122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="18">
+        <v>326882</v>
+      </c>
+      <c r="F20" s="1">
+        <v>18</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20">
+        <v>130084</v>
+      </c>
+      <c r="K20" s="1">
+        <v>18</v>
+      </c>
+      <c r="L20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20" t="s">
+        <v>15</v>
+      </c>
+      <c r="N20">
+        <v>28741</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="18">
+        <v>188639</v>
+      </c>
+      <c r="F21" s="1">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21">
+        <v>100752</v>
+      </c>
+      <c r="K21" s="1">
+        <v>19</v>
+      </c>
+      <c r="L21" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21">
+        <v>20937</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>20</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="18">
+        <v>61793</v>
+      </c>
+      <c r="F22" s="1">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22">
+        <v>72474</v>
+      </c>
+      <c r="K22" s="1">
+        <v>20</v>
+      </c>
+      <c r="L22" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" t="s">
+        <v>15</v>
+      </c>
+      <c r="N22">
+        <v>13931</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="18">
+        <v>35136</v>
+      </c>
+      <c r="F23" s="1">
+        <v>21</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23">
+        <v>1000</v>
+      </c>
+      <c r="K23" s="1">
+        <v>21</v>
+      </c>
+      <c r="L23" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23">
+        <v>50278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="18">
+        <v>100</v>
+      </c>
+      <c r="F24" s="1">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24">
+        <v>93540</v>
+      </c>
+      <c r="K24" s="1">
+        <v>22</v>
+      </c>
+      <c r="L24" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" t="s">
+        <v>15</v>
+      </c>
+      <c r="N24">
+        <v>74775</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>23</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="18">
+        <v>54485</v>
+      </c>
+      <c r="F25" s="1">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25">
+        <v>396256</v>
+      </c>
+      <c r="K25" s="1">
+        <v>23</v>
+      </c>
+      <c r="L25" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>24</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="18">
+        <v>172594</v>
+      </c>
+      <c r="F26" s="1">
+        <v>24</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26">
+        <v>2322</v>
+      </c>
+      <c r="K26" s="1">
+        <v>24</v>
+      </c>
+      <c r="L26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N26">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>25</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="18">
+        <v>3350</v>
+      </c>
+      <c r="F27" s="1">
+        <v>25</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27">
+        <v>2800</v>
+      </c>
+      <c r="K27" s="1">
+        <v>25</v>
+      </c>
+      <c r="L27" t="s">
+        <v>13</v>
+      </c>
+      <c r="M27" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27">
+        <v>16620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>26</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="18">
+        <v>1600</v>
+      </c>
+      <c r="F28" s="1">
+        <v>26</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28">
+        <v>51812</v>
+      </c>
+      <c r="K28" s="1">
+        <v>26</v>
+      </c>
+      <c r="L28" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28">
+        <v>48322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <v>27</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="18">
+        <v>52741</v>
+      </c>
+      <c r="F29" s="1">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29">
+        <v>183191</v>
+      </c>
+      <c r="K29" s="1">
+        <v>27</v>
+      </c>
+      <c r="L29" t="s">
+        <v>2</v>
+      </c>
+      <c r="M29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29">
+        <v>36683</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="19">
+        <v>28</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="21">
+        <v>124640</v>
+      </c>
+      <c r="F30" s="1">
+        <v>28</v>
+      </c>
+      <c r="G30" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30">
+        <v>94471</v>
+      </c>
+      <c r="K30" s="1">
+        <v>28</v>
+      </c>
+      <c r="L30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30">
+        <v>168998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>29</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="16">
+        <v>121871</v>
+      </c>
+      <c r="F31" s="1">
+        <v>29</v>
+      </c>
+      <c r="G31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31">
+        <v>1012124</v>
+      </c>
+      <c r="K31" s="1">
+        <v>29</v>
+      </c>
+      <c r="L31" t="s">
+        <v>5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31">
+        <v>6479</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
+        <v>30</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="18">
+        <v>385268</v>
+      </c>
+      <c r="F32" s="1">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32">
+        <v>25606</v>
+      </c>
+      <c r="K32" s="1">
+        <v>30</v>
+      </c>
+      <c r="L32" t="s">
+        <v>6</v>
+      </c>
+      <c r="M32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32">
+        <v>2576823</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
+        <v>31</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="18">
+        <v>7556</v>
+      </c>
+      <c r="F33" s="1">
+        <v>31</v>
+      </c>
+      <c r="G33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33">
+        <v>10143433</v>
+      </c>
+      <c r="K33" s="1">
+        <v>31</v>
+      </c>
+      <c r="L33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M33" t="s">
+        <v>16</v>
+      </c>
+      <c r="N33">
+        <v>885373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>32</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="18">
+        <v>5307690</v>
+      </c>
+      <c r="F34" s="1">
+        <v>32</v>
+      </c>
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34">
+        <v>3494228</v>
+      </c>
+      <c r="K34" s="1">
+        <v>32</v>
+      </c>
+      <c r="L34" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N34">
+        <v>182891</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
+        <v>33</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="18">
+        <v>1943080</v>
+      </c>
+      <c r="F35" s="1">
+        <v>33</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35">
+        <v>884109</v>
+      </c>
+      <c r="K35" s="1">
+        <v>33</v>
+      </c>
+      <c r="L35" t="s">
+        <v>8</v>
+      </c>
+      <c r="M35" t="s">
+        <v>16</v>
+      </c>
+      <c r="N35">
+        <v>665565</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>34</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="18">
+        <v>570744</v>
+      </c>
+      <c r="F36" s="1">
+        <v>34</v>
+      </c>
+      <c r="G36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36">
+        <v>1721840</v>
+      </c>
+      <c r="K36" s="1">
+        <v>34</v>
+      </c>
+      <c r="L36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" t="s">
+        <v>16</v>
+      </c>
+      <c r="N36">
+        <v>718679</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
+        <v>35</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="18">
+        <v>925408</v>
+      </c>
+      <c r="F37" s="1">
+        <v>35</v>
+      </c>
+      <c r="G37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37">
+        <v>7900</v>
+      </c>
+      <c r="K37" s="1">
+        <v>35</v>
+      </c>
+      <c r="L37" t="s">
+        <v>10</v>
+      </c>
+      <c r="M37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N37">
+        <v>1473538</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
+        <v>36</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="18">
+        <v>15770</v>
+      </c>
+      <c r="F38" s="1">
+        <v>36</v>
+      </c>
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38">
+        <v>1937555</v>
+      </c>
+      <c r="K38" s="1">
+        <v>36</v>
+      </c>
+      <c r="L38" t="s">
+        <v>11</v>
+      </c>
+      <c r="M38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
+        <v>37</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1271644</v>
+      </c>
+      <c r="F39" s="1">
+        <v>37</v>
+      </c>
+      <c r="G39" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39">
+        <v>3621443</v>
+      </c>
+      <c r="K39" s="1">
+        <v>37</v>
+      </c>
+      <c r="L39" t="s">
+        <v>12</v>
+      </c>
+      <c r="M39" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39">
+        <v>31036</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
+        <v>38</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="18">
+        <v>1848972</v>
+      </c>
+      <c r="F40" s="1">
+        <v>38</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40">
+        <v>24600</v>
+      </c>
+      <c r="K40" s="1">
+        <v>38</v>
+      </c>
+      <c r="L40" t="s">
+        <v>13</v>
+      </c>
+      <c r="M40" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40">
+        <v>147598</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="17">
+        <v>39</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="18">
+        <v>239877</v>
+      </c>
+      <c r="F41" s="1">
+        <v>39</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41">
+        <v>100383</v>
+      </c>
+      <c r="K41" s="1">
+        <v>39</v>
+      </c>
+      <c r="L41" t="s">
+        <v>14</v>
+      </c>
+      <c r="M41" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41">
+        <v>676520</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
+        <v>40</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="18">
+        <v>65200</v>
+      </c>
+      <c r="F42" s="1">
+        <v>40</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42">
+        <v>377699</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>41</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="18">
+        <v>193871</v>
+      </c>
+      <c r="F43" s="1">
+        <v>41</v>
+      </c>
+      <c r="G43" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43">
+        <v>3864721</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="19">
+        <v>42</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="21">
+        <v>2066044</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3661,10 +5374,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>355913050111991</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>